<commit_message>
Documentacion del proyecto Se obtienen los resultados que son reportados en el trabajo de tesis. Ruta de resultados reportados: ./img/Conjunto2/bmp/40x/_Resultados2017121
</commit_message>
<xml_diff>
--- a/ValidacionOpenComet ES.xlsx
+++ b/ValidacionOpenComet ES.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="65">
   <si>
     <t>OpenComet Original &amp; Modificado</t>
   </si>
@@ -217,13 +217,16 @@
   </si>
   <si>
     <t>HRatio Máximo</t>
+  </si>
+  <si>
+    <t>CORRECTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +260,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00000A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -387,6 +397,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,29 +433,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,7 +719,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,45 +736,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="E1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="E1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="31" t="s">
+      <c r="B2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="1"/>
@@ -777,19 +790,19 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="3">
@@ -803,11 +816,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
       <c r="E5" s="7"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -823,13 +836,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="25">
         <v>400</v>
       </c>
       <c r="E6" s="7"/>
@@ -839,13 +852,13 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="25">
         <v>0.85</v>
       </c>
       <c r="E7" s="7" t="b">
@@ -865,13 +878,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="25">
         <v>0.5</v>
       </c>
       <c r="E8" s="2"/>
@@ -889,13 +902,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="25">
         <v>1.05</v>
       </c>
       <c r="E9" s="2"/>
@@ -905,11 +918,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -925,13 +938,13 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="25">
         <v>0.15</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -952,13 +965,13 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="25">
         <v>0.2</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -979,20 +992,20 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1015,7 +1028,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,29 +1051,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="20"/>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
       <c r="H1" s="18"/>
-      <c r="I1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="I1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
       <c r="M1" s="6"/>
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1070,7 +1083,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="23" t="s">
         <v>50</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1080,17 +1093,17 @@
         <v>15</v>
       </c>
       <c r="H2" s="8"/>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
       <c r="O2" s="10"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1100,7 +1113,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="23" t="s">
         <v>51</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -1124,7 +1137,7 @@
       <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1134,7 +1147,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="9"/>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -1164,17 +1177,17 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="18"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
@@ -1194,7 +1207,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1204,7 +1217,7 @@
         <v>400</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="23" t="s">
         <v>53</v>
       </c>
       <c r="F6" s="7" t="s">
@@ -1222,7 +1235,7 @@
       <c r="O6" s="12"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1232,7 +1245,7 @@
         <v>0.85</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="23" t="s">
         <v>61</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -1262,7 +1275,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1272,7 +1285,7 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="23" t="s">
         <v>62</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -1300,7 +1313,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1310,7 +1323,7 @@
         <v>1.05</v>
       </c>
       <c r="D9" s="8"/>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="23" t="s">
         <v>63</v>
       </c>
       <c r="F9" s="7" t="s">
@@ -1328,17 +1341,17 @@
       <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="20"/>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="18"/>
       <c r="I10" s="2" t="s">
         <v>4</v>
@@ -1354,7 +1367,7 @@
       <c r="O10" s="8"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1364,7 +1377,7 @@
         <v>0.15</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="23" t="s">
         <v>57</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -1393,7 +1406,7 @@
       <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1403,7 +1416,7 @@
         <v>0.2</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="23" t="s">
         <v>58</v>
       </c>
       <c r="F12" s="7" t="s">
@@ -1432,22 +1445,22 @@
       <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="20"/>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="19"/>
       <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="23" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1457,7 +1470,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="23" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="7" t="s">
@@ -1473,11 +1486,11 @@
       <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
@@ -1485,7 +1498,7 @@
       <c r="O16" s="8"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1501,7 +1514,7 @@
       <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1517,7 +1530,7 @@
       <c r="O18" s="8"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1533,11 +1546,11 @@
       <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
@@ -1545,7 +1558,7 @@
       <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1561,7 +1574,7 @@
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1577,7 +1590,7 @@
       <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1593,7 +1606,7 @@
       <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1609,11 +1622,11 @@
       <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
@@ -1621,7 +1634,7 @@
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -1637,7 +1650,7 @@
       <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -1653,11 +1666,11 @@
       <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
@@ -1665,7 +1678,7 @@
       <c r="O28" s="8"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -1712,6 +1725,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="I2:M2"/>
@@ -1721,11 +1739,6 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1754,17 +1767,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="E1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1777,13 +1790,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1830,11 +1843,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="E5" s="7"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -1926,11 +1939,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1992,11 +2005,11 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2044,17 +2057,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="E1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2067,13 +2080,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2120,11 +2133,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -2216,11 +2229,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2252,7 +2265,7 @@
         <v>45</v>
       </c>
       <c r="H11" s="15">
-        <f t="shared" ref="H11:I11" si="0">((100*H4)/(H4+H8))</f>
+        <f t="shared" ref="H11" si="0">((100*H4)/(H4+H8))</f>
         <v>90</v>
       </c>
       <c r="I11" s="15"/>
@@ -2276,17 +2289,17 @@
         <v>0</v>
       </c>
       <c r="H12" s="15">
-        <f t="shared" ref="H12:I12" si="1">((100*H5)/(H5+H7))</f>
+        <f t="shared" ref="H12" si="1">((100*H5)/(H5+H7))</f>
         <v>0</v>
       </c>
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2334,17 +2347,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="E1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2357,13 +2370,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2410,11 +2423,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -2506,11 +2519,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2542,7 +2555,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="15">
-        <f t="shared" ref="H11:I11" si="0">((100*H4)/(H4+H8))</f>
+        <f t="shared" ref="H11" si="0">((100*H4)/(H4+H8))</f>
         <v>35</v>
       </c>
       <c r="I11" s="15"/>
@@ -2566,17 +2579,17 @@
         <v>0</v>
       </c>
       <c r="H12" s="15">
-        <f t="shared" ref="H12:I12" si="1">((100*H5)/(H5+H7))</f>
+        <f t="shared" ref="H12" si="1">((100*H5)/(H5+H7))</f>
         <v>0</v>
       </c>
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2624,17 +2637,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="E1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2647,13 +2660,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2700,11 +2713,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -2796,11 +2809,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2832,7 +2845,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="15">
-        <f t="shared" ref="H11:I11" si="0">((100*H4)/(H4+H8))</f>
+        <f t="shared" ref="H11" si="0">((100*H4)/(H4+H8))</f>
         <v>35</v>
       </c>
       <c r="I11" s="15"/>
@@ -2856,17 +2869,17 @@
         <v>0</v>
       </c>
       <c r="H12" s="15">
-        <f t="shared" ref="H12:I12" si="1">((100*H5)/(H5+H7))</f>
+        <f t="shared" ref="H12" si="1">((100*H5)/(H5+H7))</f>
         <v>0</v>
       </c>
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2914,17 +2927,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="E1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2937,13 +2950,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2990,11 +3003,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -3086,11 +3099,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -3122,7 +3135,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="15">
-        <f t="shared" ref="H11:I11" si="0">((100*H4)/(H4+H8))</f>
+        <f t="shared" ref="H11" si="0">((100*H4)/(H4+H8))</f>
         <v>35</v>
       </c>
       <c r="I11" s="15"/>
@@ -3146,17 +3159,17 @@
         <v>0</v>
       </c>
       <c r="H12" s="15">
-        <f t="shared" ref="H12:I12" si="1">((100*H5)/(H5+H7))</f>
+        <f t="shared" ref="H12" si="1">((100*H5)/(H5+H7))</f>
         <v>0</v>
       </c>
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">

</xml_diff>